<commit_message>
Fix go demo example
</commit_message>
<xml_diff>
--- a/examples/array-map/新手任务.xlsx
+++ b/examples/array-map/新手任务.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -217,10 +217,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>=&amp;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Food=10&amp;Gas=100</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -267,6 +263,10 @@
   </si>
   <si>
     <t>+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&amp;=</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -703,10 +703,10 @@
         <v>4</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>1</v>
@@ -723,10 +723,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>5</v>
@@ -743,10 +743,10 @@
         <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
@@ -763,10 +763,10 @@
         <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>12</v>
@@ -783,10 +783,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>15</v>
@@ -803,10 +803,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>17</v>
@@ -823,10 +823,10 @@
         <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>19</v>
@@ -843,10 +843,10 @@
         <v>24</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>22</v>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -925,7 +925,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
         <v>52</v>
@@ -936,7 +936,7 @@
         <v>51</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
         <v>53</v>

</xml_diff>